<commit_message>
upload the results of sc
</commit_message>
<xml_diff>
--- a/results_sc/500/cifar100-500samples-500groups-sc-bim.xlsx
+++ b/results_sc/500/cifar100-500samples-500groups-sc-bim.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Elements/AnonymousRep01/results_sc/500/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuzhuo/AnonymousRep01/results_sc/500/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:SF10"/>
+  <dimension ref="A1:SF9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="RQ1" workbookViewId="0">
-      <selection activeCell="A10" activeCellId="1" sqref="A4:XFD4 A10:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -6377,1508 +6377,6 @@
         <v>0.114929432111001</v>
       </c>
     </row>
-    <row r="10" spans="1:500" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>0.58928421970366329</v>
-      </c>
-      <c r="B10">
-        <v>0.12901929087669281</v>
-      </c>
-      <c r="C10">
-        <v>5.7135780883225802E-2</v>
-      </c>
-      <c r="D10">
-        <v>0.5333061278541309</v>
-      </c>
-      <c r="E10">
-        <v>7.4406917142500806E-2</v>
-      </c>
-      <c r="F10">
-        <v>0.59707761449756724</v>
-      </c>
-      <c r="G10">
-        <v>0.71253395984264745</v>
-      </c>
-      <c r="H10">
-        <v>0.33202477698343558</v>
-      </c>
-      <c r="I10">
-        <v>9.1053228586203905E-2</v>
-      </c>
-      <c r="J10">
-        <v>0.66433032306713602</v>
-      </c>
-      <c r="K10">
-        <v>0.71045416982333787</v>
-      </c>
-      <c r="L10">
-        <v>0.73294118806803044</v>
-      </c>
-      <c r="M10">
-        <v>0.6097815285969489</v>
-      </c>
-      <c r="N10">
-        <v>0.20772053815670219</v>
-      </c>
-      <c r="O10">
-        <v>0.6492367190132986</v>
-      </c>
-      <c r="P10">
-        <v>1.2154812353953881E-3</v>
-      </c>
-      <c r="Q10">
-        <v>0.36457859721755848</v>
-      </c>
-      <c r="R10">
-        <v>0.75421557328156541</v>
-      </c>
-      <c r="S10">
-        <v>3.6776210271387437E-2</v>
-      </c>
-      <c r="T10">
-        <v>0.98900478395887559</v>
-      </c>
-      <c r="U10">
-        <v>9.7500794453989403E-2</v>
-      </c>
-      <c r="V10">
-        <v>0.48329936727535078</v>
-      </c>
-      <c r="W10">
-        <v>0.97239402438788014</v>
-      </c>
-      <c r="X10">
-        <v>0.93146528693171038</v>
-      </c>
-      <c r="Y10">
-        <v>0.84529286881898424</v>
-      </c>
-      <c r="Z10">
-        <v>0.85789020248046166</v>
-      </c>
-      <c r="AA10">
-        <v>0.30785283298948651</v>
-      </c>
-      <c r="AB10">
-        <v>0.32431476650136581</v>
-      </c>
-      <c r="AC10">
-        <v>0.69571641314379218</v>
-      </c>
-      <c r="AD10">
-        <v>0.49646908331221012</v>
-      </c>
-      <c r="AE10">
-        <v>0.68040536121797224</v>
-      </c>
-      <c r="AF10">
-        <v>0.15259900007088151</v>
-      </c>
-      <c r="AG10">
-        <v>0.74219043966847886</v>
-      </c>
-      <c r="AH10">
-        <v>0.49915410882381761</v>
-      </c>
-      <c r="AI10">
-        <v>0.34660601352909459</v>
-      </c>
-      <c r="AJ10">
-        <v>4.89046427159745E-2</v>
-      </c>
-      <c r="AK10">
-        <v>0.32058563985983302</v>
-      </c>
-      <c r="AL10">
-        <v>0.58450535939977311</v>
-      </c>
-      <c r="AM10">
-        <v>0.24929314011604969</v>
-      </c>
-      <c r="AN10">
-        <v>0.65015692804470337</v>
-      </c>
-      <c r="AO10">
-        <v>0.6300293380129397</v>
-      </c>
-      <c r="AP10">
-        <v>0.43756772559505719</v>
-      </c>
-      <c r="AQ10">
-        <v>0.61384273307574766</v>
-      </c>
-      <c r="AR10">
-        <v>0.88180923755094909</v>
-      </c>
-      <c r="AS10">
-        <v>0.3545721999598529</v>
-      </c>
-      <c r="AT10">
-        <v>0.4265747596676186</v>
-      </c>
-      <c r="AU10">
-        <v>0.74255749648446712</v>
-      </c>
-      <c r="AV10">
-        <v>0.1457178645721687</v>
-      </c>
-      <c r="AW10">
-        <v>0.29757414702136281</v>
-      </c>
-      <c r="AX10">
-        <v>0.38093382608608523</v>
-      </c>
-      <c r="AY10">
-        <v>0.47364355315825579</v>
-      </c>
-      <c r="AZ10">
-        <v>0.89192277186690105</v>
-      </c>
-      <c r="BA10">
-        <v>0.114929432111001</v>
-      </c>
-      <c r="BB10">
-        <v>0.49568206926688829</v>
-      </c>
-      <c r="BC10">
-        <v>0.53007467387280349</v>
-      </c>
-      <c r="BD10">
-        <v>0.55406722771732053</v>
-      </c>
-      <c r="BE10">
-        <v>0.32468123431987878</v>
-      </c>
-      <c r="BF10">
-        <v>8.9522826492374197E-2</v>
-      </c>
-      <c r="BG10">
-        <v>0.21063104973179481</v>
-      </c>
-      <c r="BH10">
-        <v>0.2100047658921386</v>
-      </c>
-      <c r="BI10">
-        <v>0.80903728810387521</v>
-      </c>
-      <c r="BJ10">
-        <v>0.43162250875138108</v>
-      </c>
-      <c r="BK10">
-        <v>7.1426026136351739E-2</v>
-      </c>
-      <c r="BL10">
-        <v>0.21278219541207491</v>
-      </c>
-      <c r="BM10">
-        <v>0.53135775355636672</v>
-      </c>
-      <c r="BN10">
-        <v>0.32646186192547322</v>
-      </c>
-      <c r="BO10">
-        <v>0.26564428461735567</v>
-      </c>
-      <c r="BP10">
-        <v>3.5578699711186768E-2</v>
-      </c>
-      <c r="BQ10">
-        <v>0.75231205622524111</v>
-      </c>
-      <c r="BR10">
-        <v>0.83838753649651254</v>
-      </c>
-      <c r="BS10">
-        <v>0.78951926795923</v>
-      </c>
-      <c r="BT10">
-        <v>0.80249887136051412</v>
-      </c>
-      <c r="BU10">
-        <v>0.45057271003729732</v>
-      </c>
-      <c r="BV10">
-        <v>0.19553145041696679</v>
-      </c>
-      <c r="BW10">
-        <v>0.34196186196718859</v>
-      </c>
-      <c r="BX10">
-        <v>0.38463736873133608</v>
-      </c>
-      <c r="BY10">
-        <v>0.95408256844514627</v>
-      </c>
-      <c r="BZ10">
-        <v>0.81852449923702897</v>
-      </c>
-      <c r="CA10">
-        <v>0.8646539325215753</v>
-      </c>
-      <c r="CB10">
-        <v>0.16549653047910279</v>
-      </c>
-      <c r="CC10">
-        <v>0.25165691801009232</v>
-      </c>
-      <c r="CD10">
-        <v>0.50936034624014292</v>
-      </c>
-      <c r="CE10">
-        <v>2.523717232522249E-2</v>
-      </c>
-      <c r="CF10">
-        <v>0.82796767463132759</v>
-      </c>
-      <c r="CG10">
-        <v>0.25083031836427661</v>
-      </c>
-      <c r="CH10">
-        <v>0.4340273348357151</v>
-      </c>
-      <c r="CI10">
-        <v>0.72762520581422607</v>
-      </c>
-      <c r="CJ10">
-        <v>0.78813358902784536</v>
-      </c>
-      <c r="CK10">
-        <v>0.21749628543821839</v>
-      </c>
-      <c r="CL10">
-        <v>0.81033740976391944</v>
-      </c>
-      <c r="CM10">
-        <v>2.532771058314098E-2</v>
-      </c>
-      <c r="CN10">
-        <v>0.88445666743758866</v>
-      </c>
-      <c r="CO10">
-        <v>0.82536110331375057</v>
-      </c>
-      <c r="CP10">
-        <v>0.85874123503403577</v>
-      </c>
-      <c r="CQ10">
-        <v>0.1971130188647485</v>
-      </c>
-      <c r="CR10">
-        <v>0.40842090812503951</v>
-      </c>
-      <c r="CS10">
-        <v>4.8638079451172711E-2</v>
-      </c>
-      <c r="CT10">
-        <v>0.75066399182224464</v>
-      </c>
-      <c r="CU10">
-        <v>0.81935565227038953</v>
-      </c>
-      <c r="CV10">
-        <v>0.9367512179281372</v>
-      </c>
-      <c r="CW10">
-        <v>0.78789477454324952</v>
-      </c>
-      <c r="CX10">
-        <v>0.80049564620511304</v>
-      </c>
-      <c r="CY10">
-        <v>0.99624141522272891</v>
-      </c>
-      <c r="CZ10">
-        <v>0.48206873925645549</v>
-      </c>
-      <c r="DA10">
-        <v>1.735738046340618E-2</v>
-      </c>
-      <c r="DB10">
-        <v>0.30095683933235567</v>
-      </c>
-      <c r="DC10">
-        <v>0.2227154564077761</v>
-      </c>
-      <c r="DD10">
-        <v>7.6802888689927129E-2</v>
-      </c>
-      <c r="DE10">
-        <v>0.32958102600643768</v>
-      </c>
-      <c r="DF10">
-        <v>0.68357221050261374</v>
-      </c>
-      <c r="DG10">
-        <v>0.1424269570129417</v>
-      </c>
-      <c r="DH10">
-        <v>0.1871289112940763</v>
-      </c>
-      <c r="DI10">
-        <v>0.88409896050414083</v>
-      </c>
-      <c r="DJ10">
-        <v>0.897522354986242</v>
-      </c>
-      <c r="DK10">
-        <v>0.62007418211097098</v>
-      </c>
-      <c r="DL10">
-        <v>1.3084488322380849E-2</v>
-      </c>
-      <c r="DM10">
-        <v>0.6267179575934323</v>
-      </c>
-      <c r="DN10">
-        <v>0.86252943312772079</v>
-      </c>
-      <c r="DO10">
-        <v>0.28024056325108232</v>
-      </c>
-      <c r="DP10">
-        <v>0.88988833554988478</v>
-      </c>
-      <c r="DQ10">
-        <v>0.98370139227046749</v>
-      </c>
-      <c r="DR10">
-        <v>0.90231261574724486</v>
-      </c>
-      <c r="DS10">
-        <v>0.89315408717008293</v>
-      </c>
-      <c r="DT10">
-        <v>5.6048953551256719E-2</v>
-      </c>
-      <c r="DU10">
-        <v>0.32410065085476952</v>
-      </c>
-      <c r="DV10">
-        <v>0.72495618520294758</v>
-      </c>
-      <c r="DW10">
-        <v>7.3442818898483031E-2</v>
-      </c>
-      <c r="DX10">
-        <v>0.45835350182029949</v>
-      </c>
-      <c r="DY10">
-        <v>0.46404659442640372</v>
-      </c>
-      <c r="DZ10">
-        <v>6.5632749079340136E-2</v>
-      </c>
-      <c r="EA10">
-        <v>0.83820853897067404</v>
-      </c>
-      <c r="EB10">
-        <v>5.9792420625074623E-2</v>
-      </c>
-      <c r="EC10">
-        <v>0.18061656970815401</v>
-      </c>
-      <c r="ED10">
-        <v>0.44820871032140758</v>
-      </c>
-      <c r="EE10">
-        <v>0.73445041990963089</v>
-      </c>
-      <c r="EF10">
-        <v>0.12055182092811741</v>
-      </c>
-      <c r="EG10">
-        <v>0.30673845131314798</v>
-      </c>
-      <c r="EH10">
-        <v>0.62717193371085966</v>
-      </c>
-      <c r="EI10">
-        <v>0.28090456555568177</v>
-      </c>
-      <c r="EJ10">
-        <v>8.4683227468297373E-2</v>
-      </c>
-      <c r="EK10">
-        <v>0.49947789342499022</v>
-      </c>
-      <c r="EL10">
-        <v>0.71566803451012884</v>
-      </c>
-      <c r="EM10">
-        <v>0.87966364369007854</v>
-      </c>
-      <c r="EN10">
-        <v>0.82113269390919963</v>
-      </c>
-      <c r="EO10">
-        <v>0.24146336755500161</v>
-      </c>
-      <c r="EP10">
-        <v>0.23480487352439169</v>
-      </c>
-      <c r="EQ10">
-        <v>0.9973966294433867</v>
-      </c>
-      <c r="ER10">
-        <v>0.61569141558407614</v>
-      </c>
-      <c r="ES10">
-        <v>0.99470444102432076</v>
-      </c>
-      <c r="ET10">
-        <v>0.90049066719805848</v>
-      </c>
-      <c r="EU10">
-        <v>0.83499543141820043</v>
-      </c>
-      <c r="EV10">
-        <v>0.25331118225275068</v>
-      </c>
-      <c r="EW10">
-        <v>0.54662866739625493</v>
-      </c>
-      <c r="EX10">
-        <v>0.26187515249997861</v>
-      </c>
-      <c r="EY10">
-        <v>0.82294606456194008</v>
-      </c>
-      <c r="EZ10">
-        <v>0.44342734353130181</v>
-      </c>
-      <c r="FA10">
-        <v>0.21612494087996079</v>
-      </c>
-      <c r="FB10">
-        <v>0.75643183529567304</v>
-      </c>
-      <c r="FC10">
-        <v>0.23013858747228511</v>
-      </c>
-      <c r="FD10">
-        <v>0.55162505935810391</v>
-      </c>
-      <c r="FE10">
-        <v>0.53132042380239353</v>
-      </c>
-      <c r="FF10">
-        <v>0.32758633755389988</v>
-      </c>
-      <c r="FG10">
-        <v>0.20772053815670219</v>
-      </c>
-      <c r="FH10">
-        <v>0.6492367190132986</v>
-      </c>
-      <c r="FI10">
-        <v>1.2154812353953881E-3</v>
-      </c>
-      <c r="FJ10">
-        <v>0.36457859721755848</v>
-      </c>
-      <c r="FK10">
-        <v>0.75421557328156541</v>
-      </c>
-      <c r="FL10">
-        <v>3.6776210271387437E-2</v>
-      </c>
-      <c r="FM10">
-        <v>0.98900478395887559</v>
-      </c>
-      <c r="FN10">
-        <v>9.7500794453989403E-2</v>
-      </c>
-      <c r="FO10">
-        <v>0.48329936727535078</v>
-      </c>
-      <c r="FP10">
-        <v>0.97239402438788014</v>
-      </c>
-      <c r="FQ10">
-        <v>0.93146528693171038</v>
-      </c>
-      <c r="FR10">
-        <v>0.84529286881898424</v>
-      </c>
-      <c r="FS10">
-        <v>0.85789020248046166</v>
-      </c>
-      <c r="FT10">
-        <v>0.30785283298948651</v>
-      </c>
-      <c r="FU10">
-        <v>0.32431476650136581</v>
-      </c>
-      <c r="FV10">
-        <v>0.69571641314379218</v>
-      </c>
-      <c r="FW10">
-        <v>0.49646908331221012</v>
-      </c>
-      <c r="FX10">
-        <v>0.68040536121797224</v>
-      </c>
-      <c r="FY10">
-        <v>0.15259900007088151</v>
-      </c>
-      <c r="FZ10">
-        <v>0.74219043966847886</v>
-      </c>
-      <c r="GA10">
-        <v>0.49915410882381761</v>
-      </c>
-      <c r="GB10">
-        <v>0.34660601352909459</v>
-      </c>
-      <c r="GC10">
-        <v>4.89046427159745E-2</v>
-      </c>
-      <c r="GD10">
-        <v>0.32058563985983302</v>
-      </c>
-      <c r="GE10">
-        <v>0.58450535939977311</v>
-      </c>
-      <c r="GF10">
-        <v>0.24929314011604969</v>
-      </c>
-      <c r="GG10">
-        <v>0.65015692804470337</v>
-      </c>
-      <c r="GH10">
-        <v>0.6300293380129397</v>
-      </c>
-      <c r="GI10">
-        <v>0.43756772559505719</v>
-      </c>
-      <c r="GJ10">
-        <v>0.61384273307574766</v>
-      </c>
-      <c r="GK10">
-        <v>0.88180923755094909</v>
-      </c>
-      <c r="GL10">
-        <v>0.3545721999598529</v>
-      </c>
-      <c r="GM10">
-        <v>0.4265747596676186</v>
-      </c>
-      <c r="GN10">
-        <v>0.74255749648446712</v>
-      </c>
-      <c r="GO10">
-        <v>0.1457178645721687</v>
-      </c>
-      <c r="GP10">
-        <v>0.29757414702136281</v>
-      </c>
-      <c r="GQ10">
-        <v>0.38093382608608523</v>
-      </c>
-      <c r="GR10">
-        <v>0.47364355315825579</v>
-      </c>
-      <c r="GS10">
-        <v>0.89192277186690105</v>
-      </c>
-      <c r="GT10">
-        <v>0.114929432111001</v>
-      </c>
-      <c r="GU10">
-        <v>0.49568206926688829</v>
-      </c>
-      <c r="GV10">
-        <v>0.53007467387280349</v>
-      </c>
-      <c r="GW10">
-        <v>0.55406722771732053</v>
-      </c>
-      <c r="GX10">
-        <v>0.32468123431987878</v>
-      </c>
-      <c r="GY10">
-        <v>8.9522826492374197E-2</v>
-      </c>
-      <c r="GZ10">
-        <v>0.21063104973179481</v>
-      </c>
-      <c r="HA10">
-        <v>0.2100047658921386</v>
-      </c>
-      <c r="HB10">
-        <v>0.80903728810387521</v>
-      </c>
-      <c r="HC10">
-        <v>0.43162250875138108</v>
-      </c>
-      <c r="HD10">
-        <v>7.1426026136351739E-2</v>
-      </c>
-      <c r="HE10">
-        <v>0.21278219541207491</v>
-      </c>
-      <c r="HF10">
-        <v>0.53135775355636672</v>
-      </c>
-      <c r="HG10">
-        <v>0.32646186192547322</v>
-      </c>
-      <c r="HH10">
-        <v>0.26564428461735567</v>
-      </c>
-      <c r="HI10">
-        <v>3.5578699711186768E-2</v>
-      </c>
-      <c r="HJ10">
-        <v>0.75231205622524111</v>
-      </c>
-      <c r="HK10">
-        <v>0.83838753649651254</v>
-      </c>
-      <c r="HL10">
-        <v>0.78951926795923</v>
-      </c>
-      <c r="HM10">
-        <v>0.80249887136051412</v>
-      </c>
-      <c r="HN10">
-        <v>0.45057271003729732</v>
-      </c>
-      <c r="HO10">
-        <v>0.19553145041696679</v>
-      </c>
-      <c r="HP10">
-        <v>0.34196186196718859</v>
-      </c>
-      <c r="HQ10">
-        <v>0.38463736873133608</v>
-      </c>
-      <c r="HR10">
-        <v>0.95408256844514627</v>
-      </c>
-      <c r="HS10">
-        <v>0.81852449923702897</v>
-      </c>
-      <c r="HT10">
-        <v>0.8646539325215753</v>
-      </c>
-      <c r="HU10">
-        <v>0.16549653047910279</v>
-      </c>
-      <c r="HV10">
-        <v>0.25165691801009232</v>
-      </c>
-      <c r="HW10">
-        <v>0.50936034624014292</v>
-      </c>
-      <c r="HX10">
-        <v>2.523717232522249E-2</v>
-      </c>
-      <c r="HY10">
-        <v>0.82796767463132759</v>
-      </c>
-      <c r="HZ10">
-        <v>0.25083031836427661</v>
-      </c>
-      <c r="IA10">
-        <v>0.4340273348357151</v>
-      </c>
-      <c r="IB10">
-        <v>0.72762520581422607</v>
-      </c>
-      <c r="IC10">
-        <v>0.78813358902784536</v>
-      </c>
-      <c r="ID10">
-        <v>0.21749628543821839</v>
-      </c>
-      <c r="IE10">
-        <v>0.81033740976391944</v>
-      </c>
-      <c r="IF10">
-        <v>2.532771058314098E-2</v>
-      </c>
-      <c r="IG10">
-        <v>0.88445666743758866</v>
-      </c>
-      <c r="IH10">
-        <v>0.82536110331375057</v>
-      </c>
-      <c r="II10">
-        <v>0.85874123503403577</v>
-      </c>
-      <c r="IJ10">
-        <v>0.1971130188647485</v>
-      </c>
-      <c r="IK10">
-        <v>0.40842090812503951</v>
-      </c>
-      <c r="IL10">
-        <v>4.8638079451172711E-2</v>
-      </c>
-      <c r="IM10">
-        <v>0.75066399182224464</v>
-      </c>
-      <c r="IN10">
-        <v>0.81935565227038953</v>
-      </c>
-      <c r="IO10">
-        <v>0.9367512179281372</v>
-      </c>
-      <c r="IP10">
-        <v>0.78789477454324952</v>
-      </c>
-      <c r="IQ10">
-        <v>0.80049564620511304</v>
-      </c>
-      <c r="IR10">
-        <v>0.99624141522272891</v>
-      </c>
-      <c r="IS10">
-        <v>0.48206873925645549</v>
-      </c>
-      <c r="IT10">
-        <v>1.735738046340618E-2</v>
-      </c>
-      <c r="IU10">
-        <v>0.30095683933235567</v>
-      </c>
-      <c r="IV10">
-        <v>0.2227154564077761</v>
-      </c>
-      <c r="IW10">
-        <v>7.6802888689927129E-2</v>
-      </c>
-      <c r="IX10">
-        <v>0.32958102600643768</v>
-      </c>
-      <c r="IY10">
-        <v>0.68357221050261374</v>
-      </c>
-      <c r="IZ10">
-        <v>0.1424269570129417</v>
-      </c>
-      <c r="JA10">
-        <v>0.1871289112940763</v>
-      </c>
-      <c r="JB10">
-        <v>0.88409896050414083</v>
-      </c>
-      <c r="JC10">
-        <v>0.897522354986242</v>
-      </c>
-      <c r="JD10">
-        <v>0.62007418211097098</v>
-      </c>
-      <c r="JE10">
-        <v>1.3084488322380849E-2</v>
-      </c>
-      <c r="JF10">
-        <v>0.6267179575934323</v>
-      </c>
-      <c r="JG10">
-        <v>0.86252943312772079</v>
-      </c>
-      <c r="JH10">
-        <v>0.28024056325108232</v>
-      </c>
-      <c r="JI10">
-        <v>0.88988833554988478</v>
-      </c>
-      <c r="JJ10">
-        <v>0.98370139227046749</v>
-      </c>
-      <c r="JK10">
-        <v>0.90231261574724486</v>
-      </c>
-      <c r="JL10">
-        <v>0.89315408717008293</v>
-      </c>
-      <c r="JM10">
-        <v>5.6048953551256719E-2</v>
-      </c>
-      <c r="JN10">
-        <v>0.32410065085476952</v>
-      </c>
-      <c r="JO10">
-        <v>0.72495618520294758</v>
-      </c>
-      <c r="JP10">
-        <v>7.3442818898483031E-2</v>
-      </c>
-      <c r="JQ10">
-        <v>0.45835350182029949</v>
-      </c>
-      <c r="JR10">
-        <v>0.46404659442640372</v>
-      </c>
-      <c r="JS10">
-        <v>6.5632749079340136E-2</v>
-      </c>
-      <c r="JT10">
-        <v>0.83820853897067404</v>
-      </c>
-      <c r="JU10">
-        <v>5.9792420625074623E-2</v>
-      </c>
-      <c r="JV10">
-        <v>0.18061656970815401</v>
-      </c>
-      <c r="JW10">
-        <v>0.44820871032140758</v>
-      </c>
-      <c r="JX10">
-        <v>0.73445041990963089</v>
-      </c>
-      <c r="JY10">
-        <v>0.12055182092811741</v>
-      </c>
-      <c r="JZ10">
-        <v>0.30673845131314798</v>
-      </c>
-      <c r="KA10">
-        <v>0.62717193371085966</v>
-      </c>
-      <c r="KB10">
-        <v>0.28090456555568177</v>
-      </c>
-      <c r="KC10">
-        <v>8.4683227468297373E-2</v>
-      </c>
-      <c r="KD10">
-        <v>0.49947789342499022</v>
-      </c>
-      <c r="KE10">
-        <v>0.71566803451012884</v>
-      </c>
-      <c r="KF10">
-        <v>0.87966364369007854</v>
-      </c>
-      <c r="KG10">
-        <v>0.82113269390919963</v>
-      </c>
-      <c r="KH10">
-        <v>0.24146336755500161</v>
-      </c>
-      <c r="KI10">
-        <v>0.23480487352439169</v>
-      </c>
-      <c r="KJ10">
-        <v>0.9973966294433867</v>
-      </c>
-      <c r="KK10">
-        <v>0.61569141558407614</v>
-      </c>
-      <c r="KL10">
-        <v>0.99470444102432076</v>
-      </c>
-      <c r="KM10">
-        <v>0.90049066719805848</v>
-      </c>
-      <c r="KN10">
-        <v>0.83499543141820043</v>
-      </c>
-      <c r="KO10">
-        <v>0.25331118225275068</v>
-      </c>
-      <c r="KP10">
-        <v>0.54662866739625493</v>
-      </c>
-      <c r="KQ10">
-        <v>0.26187515249997861</v>
-      </c>
-      <c r="KR10">
-        <v>0.82294606456194008</v>
-      </c>
-      <c r="KS10">
-        <v>0.44342734353130181</v>
-      </c>
-      <c r="KT10">
-        <v>0.21612494087996079</v>
-      </c>
-      <c r="KU10">
-        <v>0.75643183529567304</v>
-      </c>
-      <c r="KV10">
-        <v>0.23013858747228511</v>
-      </c>
-      <c r="KW10">
-        <v>0.55162505935810391</v>
-      </c>
-      <c r="KX10">
-        <v>0.53132042380239353</v>
-      </c>
-      <c r="KY10">
-        <v>0.32758633755389988</v>
-      </c>
-      <c r="KZ10">
-        <v>0.20772053815670219</v>
-      </c>
-      <c r="LA10">
-        <v>0.6492367190132986</v>
-      </c>
-      <c r="LB10">
-        <v>1.2154812353953881E-3</v>
-      </c>
-      <c r="LC10">
-        <v>0.36457859721755848</v>
-      </c>
-      <c r="LD10">
-        <v>0.75421557328156541</v>
-      </c>
-      <c r="LE10">
-        <v>3.6776210271387437E-2</v>
-      </c>
-      <c r="LF10">
-        <v>0.98900478395887559</v>
-      </c>
-      <c r="LG10">
-        <v>9.7500794453989403E-2</v>
-      </c>
-      <c r="LH10">
-        <v>0.48329936727535078</v>
-      </c>
-      <c r="LI10">
-        <v>0.97239402438788014</v>
-      </c>
-      <c r="LJ10">
-        <v>0.93146528693171038</v>
-      </c>
-      <c r="LK10">
-        <v>0.84529286881898424</v>
-      </c>
-      <c r="LL10">
-        <v>0.85789020248046166</v>
-      </c>
-      <c r="LM10">
-        <v>0.30785283298948651</v>
-      </c>
-      <c r="LN10">
-        <v>0.32431476650136581</v>
-      </c>
-      <c r="LO10">
-        <v>0.69571641314379218</v>
-      </c>
-      <c r="LP10">
-        <v>0.49646908331221012</v>
-      </c>
-      <c r="LQ10">
-        <v>0.68040536121797224</v>
-      </c>
-      <c r="LR10">
-        <v>0.15259900007088151</v>
-      </c>
-      <c r="LS10">
-        <v>0.74219043966847886</v>
-      </c>
-      <c r="LT10">
-        <v>0.49915410882381761</v>
-      </c>
-      <c r="LU10">
-        <v>0.34660601352909459</v>
-      </c>
-      <c r="LV10">
-        <v>4.89046427159745E-2</v>
-      </c>
-      <c r="LW10">
-        <v>0.32058563985983302</v>
-      </c>
-      <c r="LX10">
-        <v>0.58450535939977311</v>
-      </c>
-      <c r="LY10">
-        <v>0.24929314011604969</v>
-      </c>
-      <c r="LZ10">
-        <v>0.65015692804470337</v>
-      </c>
-      <c r="MA10">
-        <v>0.6300293380129397</v>
-      </c>
-      <c r="MB10">
-        <v>0.43756772559505719</v>
-      </c>
-      <c r="MC10">
-        <v>0.61384273307574766</v>
-      </c>
-      <c r="MD10">
-        <v>0.88180923755094909</v>
-      </c>
-      <c r="ME10">
-        <v>0.3545721999598529</v>
-      </c>
-      <c r="MF10">
-        <v>0.4265747596676186</v>
-      </c>
-      <c r="MG10">
-        <v>0.74255749648446712</v>
-      </c>
-      <c r="MH10">
-        <v>0.1457178645721687</v>
-      </c>
-      <c r="MI10">
-        <v>0.29757414702136281</v>
-      </c>
-      <c r="MJ10">
-        <v>0.38093382608608523</v>
-      </c>
-      <c r="MK10">
-        <v>0.47364355315825579</v>
-      </c>
-      <c r="ML10">
-        <v>0.89192277186690105</v>
-      </c>
-      <c r="MM10">
-        <v>0.114929432111001</v>
-      </c>
-      <c r="MN10">
-        <v>0.49568206926688829</v>
-      </c>
-      <c r="MO10">
-        <v>0.53007467387280349</v>
-      </c>
-      <c r="MP10">
-        <v>0.55406722771732053</v>
-      </c>
-      <c r="MQ10">
-        <v>0.32468123431987878</v>
-      </c>
-      <c r="MR10">
-        <v>8.9522826492374197E-2</v>
-      </c>
-      <c r="MS10">
-        <v>0.21063104973179481</v>
-      </c>
-      <c r="MT10">
-        <v>0.2100047658921386</v>
-      </c>
-      <c r="MU10">
-        <v>0.80903728810387521</v>
-      </c>
-      <c r="MV10">
-        <v>0.43162250875138108</v>
-      </c>
-      <c r="MW10">
-        <v>7.1426026136351739E-2</v>
-      </c>
-      <c r="MX10">
-        <v>0.21278219541207491</v>
-      </c>
-      <c r="MY10">
-        <v>0.53135775355636672</v>
-      </c>
-      <c r="MZ10">
-        <v>0.32646186192547322</v>
-      </c>
-      <c r="NA10">
-        <v>0.26564428461735567</v>
-      </c>
-      <c r="NB10">
-        <v>3.5578699711186768E-2</v>
-      </c>
-      <c r="NC10">
-        <v>0.75231205622524111</v>
-      </c>
-      <c r="ND10">
-        <v>0.83838753649651254</v>
-      </c>
-      <c r="NE10">
-        <v>0.78951926795923</v>
-      </c>
-      <c r="NF10">
-        <v>0.80249887136051412</v>
-      </c>
-      <c r="NG10">
-        <v>0.45057271003729732</v>
-      </c>
-      <c r="NH10">
-        <v>0.19553145041696679</v>
-      </c>
-      <c r="NI10">
-        <v>0.34196186196718859</v>
-      </c>
-      <c r="NJ10">
-        <v>0.38463736873133608</v>
-      </c>
-      <c r="NK10">
-        <v>0.95408256844514627</v>
-      </c>
-      <c r="NL10">
-        <v>0.81852449923702897</v>
-      </c>
-      <c r="NM10">
-        <v>0.8646539325215753</v>
-      </c>
-      <c r="NN10">
-        <v>0.16549653047910279</v>
-      </c>
-      <c r="NO10">
-        <v>0.25165691801009232</v>
-      </c>
-      <c r="NP10">
-        <v>0.50936034624014292</v>
-      </c>
-      <c r="NQ10">
-        <v>2.523717232522249E-2</v>
-      </c>
-      <c r="NR10">
-        <v>0.82796767463132759</v>
-      </c>
-      <c r="NS10">
-        <v>0.25083031836427661</v>
-      </c>
-      <c r="NT10">
-        <v>0.4340273348357151</v>
-      </c>
-      <c r="NU10">
-        <v>0.72762520581422607</v>
-      </c>
-      <c r="NV10">
-        <v>0.78813358902784536</v>
-      </c>
-      <c r="NW10">
-        <v>0.21749628543821839</v>
-      </c>
-      <c r="NX10">
-        <v>0.81033740976391944</v>
-      </c>
-      <c r="NY10">
-        <v>2.532771058314098E-2</v>
-      </c>
-      <c r="NZ10">
-        <v>0.88445666743758866</v>
-      </c>
-      <c r="OA10">
-        <v>0.82536110331375057</v>
-      </c>
-      <c r="OB10">
-        <v>0.85874123503403577</v>
-      </c>
-      <c r="OC10">
-        <v>0.1971130188647485</v>
-      </c>
-      <c r="OD10">
-        <v>0.40842090812503951</v>
-      </c>
-      <c r="OE10">
-        <v>4.8638079451172711E-2</v>
-      </c>
-      <c r="OF10">
-        <v>0.75066399182224464</v>
-      </c>
-      <c r="OG10">
-        <v>0.81935565227038953</v>
-      </c>
-      <c r="OH10">
-        <v>0.9367512179281372</v>
-      </c>
-      <c r="OI10">
-        <v>0.78789477454324952</v>
-      </c>
-      <c r="OJ10">
-        <v>0.80049564620511304</v>
-      </c>
-      <c r="OK10">
-        <v>0.99624141522272891</v>
-      </c>
-      <c r="OL10">
-        <v>0.48206873925645549</v>
-      </c>
-      <c r="OM10">
-        <v>1.735738046340618E-2</v>
-      </c>
-      <c r="ON10">
-        <v>0.30095683933235567</v>
-      </c>
-      <c r="OO10">
-        <v>0.2227154564077761</v>
-      </c>
-      <c r="OP10">
-        <v>7.6802888689927129E-2</v>
-      </c>
-      <c r="OQ10">
-        <v>0.32958102600643768</v>
-      </c>
-      <c r="OR10">
-        <v>0.68357221050261374</v>
-      </c>
-      <c r="OS10">
-        <v>0.1424269570129417</v>
-      </c>
-      <c r="OT10">
-        <v>0.1871289112940763</v>
-      </c>
-      <c r="OU10">
-        <v>0.88409896050414083</v>
-      </c>
-      <c r="OV10">
-        <v>0.897522354986242</v>
-      </c>
-      <c r="OW10">
-        <v>0.62007418211097098</v>
-      </c>
-      <c r="OX10">
-        <v>1.3084488322380849E-2</v>
-      </c>
-      <c r="OY10">
-        <v>0.6267179575934323</v>
-      </c>
-      <c r="OZ10">
-        <v>0.86252943312772079</v>
-      </c>
-      <c r="PA10">
-        <v>0.28024056325108232</v>
-      </c>
-      <c r="PB10">
-        <v>0.88988833554988478</v>
-      </c>
-      <c r="PC10">
-        <v>0.98370139227046749</v>
-      </c>
-      <c r="PD10">
-        <v>0.90231261574724486</v>
-      </c>
-      <c r="PE10">
-        <v>0.89315408717008293</v>
-      </c>
-      <c r="PF10">
-        <v>5.6048953551256719E-2</v>
-      </c>
-      <c r="PG10">
-        <v>0.32410065085476952</v>
-      </c>
-      <c r="PH10">
-        <v>0.72495618520294758</v>
-      </c>
-      <c r="PI10">
-        <v>7.3442818898483031E-2</v>
-      </c>
-      <c r="PJ10">
-        <v>0.45835350182029949</v>
-      </c>
-      <c r="PK10">
-        <v>0.46404659442640372</v>
-      </c>
-      <c r="PL10">
-        <v>6.5632749079340136E-2</v>
-      </c>
-      <c r="PM10">
-        <v>0.83820853897067404</v>
-      </c>
-      <c r="PN10">
-        <v>5.9792420625074623E-2</v>
-      </c>
-      <c r="PO10">
-        <v>0.18061656970815401</v>
-      </c>
-      <c r="PP10">
-        <v>0.44820871032140758</v>
-      </c>
-      <c r="PQ10">
-        <v>0.73445041990963089</v>
-      </c>
-      <c r="PR10">
-        <v>0.12055182092811741</v>
-      </c>
-      <c r="PS10">
-        <v>0.30673845131314798</v>
-      </c>
-      <c r="PT10">
-        <v>0.62717193371085966</v>
-      </c>
-      <c r="PU10">
-        <v>0.28090456555568177</v>
-      </c>
-      <c r="PV10">
-        <v>8.4683227468297373E-2</v>
-      </c>
-      <c r="PW10">
-        <v>0.49947789342499022</v>
-      </c>
-      <c r="PX10">
-        <v>0.71566803451012884</v>
-      </c>
-      <c r="PY10">
-        <v>0.87966364369007854</v>
-      </c>
-      <c r="PZ10">
-        <v>0.82113269390919963</v>
-      </c>
-      <c r="QA10">
-        <v>0.24146336755500161</v>
-      </c>
-      <c r="QB10">
-        <v>0.23480487352439169</v>
-      </c>
-      <c r="QC10">
-        <v>0.9973966294433867</v>
-      </c>
-      <c r="QD10">
-        <v>0.61569141558407614</v>
-      </c>
-      <c r="QE10">
-        <v>0.99470444102432076</v>
-      </c>
-      <c r="QF10">
-        <v>0.90049066719805848</v>
-      </c>
-      <c r="QG10">
-        <v>0.83499543141820043</v>
-      </c>
-      <c r="QH10">
-        <v>0.25331118225275068</v>
-      </c>
-      <c r="QI10">
-        <v>0.54662866739625493</v>
-      </c>
-      <c r="QJ10">
-        <v>0.26187515249997861</v>
-      </c>
-      <c r="QK10">
-        <v>0.82294606456194008</v>
-      </c>
-      <c r="QL10">
-        <v>0.44342734353130181</v>
-      </c>
-      <c r="QM10">
-        <v>0.21612494087996079</v>
-      </c>
-      <c r="QN10">
-        <v>0.75643183529567304</v>
-      </c>
-      <c r="QO10">
-        <v>0.23013858747228511</v>
-      </c>
-      <c r="QP10">
-        <v>0.55162505935810391</v>
-      </c>
-      <c r="QQ10">
-        <v>0.53132042380239353</v>
-      </c>
-      <c r="QR10">
-        <v>0.32758633755389988</v>
-      </c>
-      <c r="QS10">
-        <v>0.20772053815670219</v>
-      </c>
-      <c r="QT10">
-        <v>0.6492367190132986</v>
-      </c>
-      <c r="QU10">
-        <v>1.2154812353953881E-3</v>
-      </c>
-      <c r="QV10">
-        <v>0.36457859721755848</v>
-      </c>
-      <c r="QW10">
-        <v>0.75421557328156541</v>
-      </c>
-      <c r="QX10">
-        <v>3.6776210271387437E-2</v>
-      </c>
-      <c r="QY10">
-        <v>0.98900478395887559</v>
-      </c>
-      <c r="QZ10">
-        <v>9.7500794453989403E-2</v>
-      </c>
-      <c r="RA10">
-        <v>0.48329936727535078</v>
-      </c>
-      <c r="RB10">
-        <v>0.97239402438788014</v>
-      </c>
-      <c r="RC10">
-        <v>0.93146528693171038</v>
-      </c>
-      <c r="RD10">
-        <v>0.84529286881898424</v>
-      </c>
-      <c r="RE10">
-        <v>0.85789020248046166</v>
-      </c>
-      <c r="RF10">
-        <v>0.30785283298948651</v>
-      </c>
-      <c r="RG10">
-        <v>0.32431476650136581</v>
-      </c>
-      <c r="RH10">
-        <v>0.69571641314379218</v>
-      </c>
-      <c r="RI10">
-        <v>0.49646908331221012</v>
-      </c>
-      <c r="RJ10">
-        <v>0.68040536121797224</v>
-      </c>
-      <c r="RK10">
-        <v>0.15259900007088151</v>
-      </c>
-      <c r="RL10">
-        <v>0.74219043966847886</v>
-      </c>
-      <c r="RM10">
-        <v>0.49915410882381761</v>
-      </c>
-      <c r="RN10">
-        <v>0.34660601352909459</v>
-      </c>
-      <c r="RO10">
-        <v>4.89046427159745E-2</v>
-      </c>
-      <c r="RP10">
-        <v>0.32058563985983302</v>
-      </c>
-      <c r="RQ10">
-        <v>0.58450535939977311</v>
-      </c>
-      <c r="RR10">
-        <v>0.24929314011604969</v>
-      </c>
-      <c r="RS10">
-        <v>0.65015692804470337</v>
-      </c>
-      <c r="RT10">
-        <v>0.6300293380129397</v>
-      </c>
-      <c r="RU10">
-        <v>0.43756772559505719</v>
-      </c>
-      <c r="RV10">
-        <v>0.61384273307574766</v>
-      </c>
-      <c r="RW10">
-        <v>0.88180923755094909</v>
-      </c>
-      <c r="RX10">
-        <v>0.3545721999598529</v>
-      </c>
-      <c r="RY10">
-        <v>0.4265747596676186</v>
-      </c>
-      <c r="RZ10">
-        <v>0.74255749648446712</v>
-      </c>
-      <c r="SA10">
-        <v>0.1457178645721687</v>
-      </c>
-      <c r="SB10">
-        <v>0.29757414702136281</v>
-      </c>
-      <c r="SC10">
-        <v>0.38093382608608523</v>
-      </c>
-      <c r="SD10">
-        <v>0.47364355315825579</v>
-      </c>
-      <c r="SE10">
-        <v>0.89192277186690105</v>
-      </c>
-      <c r="SF10">
-        <v>0.114929432111001</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>